<commit_message>
July 31 major cosmetic update and upload of new content.
</commit_message>
<xml_diff>
--- a/data/Euclidian_distance_demo_data.xlsx
+++ b/data/Euclidian_distance_demo_data.xlsx
@@ -1,32 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajsmit/Dropbox/R/workshops/Quantitative_Ecology/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajsmit/Documents/R_local/workshops/tangled_bank/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D95768-57F3-7047-8918-41ED14124477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE56EC62-5897-E44D-BB66-9573A58E4C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12440" yWindow="4900" windowWidth="28040" windowHeight="17440" xr2:uid="{F2E759F5-2917-7544-ABEC-A37A4335C191}"/>
+    <workbookView minimized="1" xWindow="12700" yWindow="10960" windowWidth="30360" windowHeight="25040" activeTab="2" xr2:uid="{F2E759F5-2917-7544-ABEC-A37A4335C191}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="36">
   <si>
     <t>x</t>
   </si>
@@ -65,13 +77,82 @@
   </si>
   <si>
     <t>light</t>
+  </si>
+  <si>
+    <t>site1</t>
+  </si>
+  <si>
+    <t>site2</t>
+  </si>
+  <si>
+    <t>site3</t>
+  </si>
+  <si>
+    <t>site4</t>
+  </si>
+  <si>
+    <t>site5</t>
+  </si>
+  <si>
+    <t>site6</t>
+  </si>
+  <si>
+    <t>site7</t>
+  </si>
+  <si>
+    <t>spp1</t>
+  </si>
+  <si>
+    <t>spp2</t>
+  </si>
+  <si>
+    <t>spp3</t>
+  </si>
+  <si>
+    <t>spp4</t>
+  </si>
+  <si>
+    <t>spp5</t>
+  </si>
+  <si>
+    <t>spp6</t>
+  </si>
+  <si>
+    <t>spp7</t>
+  </si>
+  <si>
+    <t>spp8</t>
+  </si>
+  <si>
+    <t>spp9</t>
+  </si>
+  <si>
+    <t>spp10</t>
+  </si>
+  <si>
+    <t>var1</t>
+  </si>
+  <si>
+    <t>var2</t>
+  </si>
+  <si>
+    <t>var3</t>
+  </si>
+  <si>
+    <t>var4</t>
+  </si>
+  <si>
+    <t>var5</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -79,16 +160,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -96,12 +218,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,9 +284,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -160,7 +324,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -266,7 +430,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,7 +572,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -418,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB7EDC6-A051-564E-AA1F-345EA266CF10}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -660,4 +824,1584 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76F4D51-C08E-8D4D-BE45-E701A4232D08}">
+  <dimension ref="B2:Z48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="6" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.6640625" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="3.6640625" customWidth="1"/>
+    <col min="21" max="21" width="6" customWidth="1"/>
+    <col min="22" max="26" width="3.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:26" ht="36" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12">
+        <v>1</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12">
+        <v>0</v>
+      </c>
+      <c r="K3" s="12">
+        <v>1</v>
+      </c>
+      <c r="L3" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0</v>
+      </c>
+      <c r="J4" s="12">
+        <v>1</v>
+      </c>
+      <c r="K4" s="12">
+        <v>1</v>
+      </c>
+      <c r="L4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <v>1</v>
+      </c>
+      <c r="I7" s="12">
+        <v>1</v>
+      </c>
+      <c r="J7" s="12">
+        <v>1</v>
+      </c>
+      <c r="K7" s="12">
+        <v>1</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12">
+        <v>1</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <v>1</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <v>0</v>
+      </c>
+      <c r="L9" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26" ht="28" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="S11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" s="1"/>
+      <c r="V11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="W11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="X11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z11" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="13">
+        <v>23</v>
+      </c>
+      <c r="D12" s="13">
+        <v>455</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
+        <v>6</v>
+      </c>
+      <c r="G12" s="13">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="N12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="13">
+        <f>(C12-AVERAGE(C$12:C$18))/STDEV(C$12:C$18)</f>
+        <v>0.15526475085202987</v>
+      </c>
+      <c r="P12" s="13">
+        <f>(D12-AVERAGE(D$12:D$18))/STDEV(D$12:D$18)</f>
+        <v>1.5179877590067181</v>
+      </c>
+      <c r="Q12" s="13">
+        <f>(E12-AVERAGE(E$12:E$18))/STDEV(E$12:E$18)</f>
+        <v>-0.58554004376912006</v>
+      </c>
+      <c r="R12" s="13">
+        <f>(F12-AVERAGE(F$12:F$18))/STDEV(F$12:F$18)</f>
+        <v>0.44908871313907145</v>
+      </c>
+      <c r="S12" s="13">
+        <f>(G12-AVERAGE(G$12:G$18))/STDEV(G$12:G$18)</f>
+        <v>-0.63719309286430925</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="V12" s="13">
+        <v>1</v>
+      </c>
+      <c r="W12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="X12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z12" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="13">
+        <v>25</v>
+      </c>
+      <c r="D13" s="13">
+        <v>345</v>
+      </c>
+      <c r="E13" s="13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="13">
+        <v>5</v>
+      </c>
+      <c r="G13" s="13">
+        <v>11</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="N13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="13">
+        <f t="shared" ref="O13:S18" si="0">(C13-AVERAGE(C$12:C$18))/STDEV(C$12:C$18)</f>
+        <v>0.5175491695067661</v>
+      </c>
+      <c r="P13" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.9795562034616011</v>
+      </c>
+      <c r="Q13" s="13">
+        <f t="shared" si="0"/>
+        <v>1.4638501094227994</v>
+      </c>
+      <c r="R13" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.33681653485430396</v>
+      </c>
+      <c r="S13" s="13">
+        <f t="shared" si="0"/>
+        <v>0.10619884881071777</v>
+      </c>
+      <c r="U13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V13" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="W13" s="13">
+        <v>1</v>
+      </c>
+      <c r="X13" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y13" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z13" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="13">
+        <v>19</v>
+      </c>
+      <c r="D14" s="13">
+        <v>421</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
+        <v>3</v>
+      </c>
+      <c r="G14" s="13">
+        <v>13</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="N14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.56930408645744246</v>
+      </c>
+      <c r="P14" s="13">
+        <f t="shared" si="0"/>
+        <v>0.74601962515287401</v>
+      </c>
+      <c r="Q14" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.58554004376912006</v>
+      </c>
+      <c r="R14" s="13">
+        <f t="shared" si="0"/>
+        <v>-1.9086270308410549</v>
+      </c>
+      <c r="S14" s="13">
+        <f t="shared" si="0"/>
+        <v>1.5929827321607717</v>
+      </c>
+      <c r="U14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="V14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="W14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="X14" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z14" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="13">
+        <v>13</v>
+      </c>
+      <c r="D15" s="13">
+        <v>329</v>
+      </c>
+      <c r="E15" s="13">
+        <v>2</v>
+      </c>
+      <c r="F15" s="13">
+        <v>6</v>
+      </c>
+      <c r="G15" s="13">
+        <v>9</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="N15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O15" s="13">
+        <f t="shared" si="0"/>
+        <v>-1.6561573424216509</v>
+      </c>
+      <c r="P15" s="13">
+        <f t="shared" si="0"/>
+        <v>-1.3428353252751748</v>
+      </c>
+      <c r="Q15" s="13">
+        <f t="shared" si="0"/>
+        <v>1.4638501094227994</v>
+      </c>
+      <c r="R15" s="13">
+        <f t="shared" si="0"/>
+        <v>0.44908871313907145</v>
+      </c>
+      <c r="S15" s="13">
+        <f t="shared" si="0"/>
+        <v>-1.3805850345393362</v>
+      </c>
+      <c r="U15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="V15" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="W15" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="X15" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y15" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="13">
+        <v>21</v>
+      </c>
+      <c r="D16" s="13">
+        <v>401</v>
+      </c>
+      <c r="E16" s="13">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13">
+        <v>7</v>
+      </c>
+      <c r="G16" s="13">
+        <v>10</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="N16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.20701966780270631</v>
+      </c>
+      <c r="P16" s="13">
+        <f t="shared" si="0"/>
+        <v>0.29192072288590692</v>
+      </c>
+      <c r="Q16" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.58554004376912006</v>
+      </c>
+      <c r="R16" s="13">
+        <f t="shared" si="0"/>
+        <v>1.234993961132447</v>
+      </c>
+      <c r="S16" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.63719309286430925</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="V16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="W16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="X16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z16" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="13">
+        <v>23</v>
+      </c>
+      <c r="D17" s="13">
+        <v>367</v>
+      </c>
+      <c r="E17" s="13">
+        <v>1</v>
+      </c>
+      <c r="F17" s="13">
+        <v>5</v>
+      </c>
+      <c r="G17" s="13">
+        <v>11</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="N17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O17" s="13">
+        <f t="shared" si="0"/>
+        <v>0.15526475085202987</v>
+      </c>
+      <c r="P17" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.48004741096793724</v>
+      </c>
+      <c r="Q17" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.58554004376912006</v>
+      </c>
+      <c r="R17" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.33681653485430396</v>
+      </c>
+      <c r="S17" s="13">
+        <f t="shared" si="0"/>
+        <v>0.10619884881071777</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="13">
+        <v>31</v>
+      </c>
+      <c r="D18" s="13">
+        <v>399</v>
+      </c>
+      <c r="E18" s="13">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13">
+        <v>6</v>
+      </c>
+      <c r="G18" s="13">
+        <v>12</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="N18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="13">
+        <f t="shared" si="0"/>
+        <v>1.6044024254709746</v>
+      </c>
+      <c r="P18" s="13">
+        <f t="shared" si="0"/>
+        <v>0.2465108326592102</v>
+      </c>
+      <c r="Q18" s="13">
+        <f t="shared" si="0"/>
+        <v>-0.58554004376912006</v>
+      </c>
+      <c r="R18" s="13">
+        <f t="shared" si="0"/>
+        <v>0.44908871313907145</v>
+      </c>
+      <c r="S18" s="13">
+        <f t="shared" si="0"/>
+        <v>0.84959079048574482</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" ht="36" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="C20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="12">
+        <v>0</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B25" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="12">
+        <v>0</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B28" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="12">
+        <v>0</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B29" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" s="12">
+        <v>0</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" ht="31" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+      <c r="C32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="12">
+        <v>0</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G37" s="12">
+        <v>0</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" s="12">
+        <v>0</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I39" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="31" x14ac:dyDescent="0.2">
+      <c r="B41" s="1"/>
+      <c r="C41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="13">
+        <v>0</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="13">
+        <v>0</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E44" s="13">
+        <v>0</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" s="13">
+        <v>0</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G46" s="13">
+        <v>0</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H47" s="13">
+        <v>0</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I48" s="13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>